<commit_message>
finalize docs and comments in code before sprint review 2
</commit_message>
<xml_diff>
--- a/documentation/Sprint 2 Tests.xlsx
+++ b/documentation/Sprint 2 Tests.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\Desktop\NCAA-Bracket-Predictor\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnh\Desktop\NCAA-Bracket-Predictor\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA2403C5-2E12-42AE-9DE0-24B99F935FE7}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A48BCB-CB63-4845-98C1-26AF5792A1AA}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5628" xr2:uid="{9DF9FD2C-CE41-44D9-B248-E86D16A5E2AD}"/>
   </bookViews>
@@ -654,20 +654,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50E2C35C-2831-4627-8391-15309EF4B4D5}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="49" customWidth="1"/>
     <col min="2" max="2" width="50" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.5234375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1015625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -684,7 +684,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -701,7 +701,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -718,7 +718,7 @@
         <v>43172</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -735,7 +735,7 @@
         <v>43172</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -752,7 +752,7 @@
         <v>43173</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -769,7 +769,7 @@
         <v>43173</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -786,7 +786,7 @@
         <v>43173</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -803,7 +803,7 @@
         <v>43173</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -820,15 +820,15 @@
         <v>43173</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A11" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -845,7 +845,7 @@
         <v>43174</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>49</v>
       </c>
@@ -862,7 +862,7 @@
         <v>43174</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>54</v>
       </c>
@@ -879,10 +879,10 @@
         <v>43174</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>57</v>
       </c>
@@ -899,7 +899,7 @@
         <v>43175</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>61</v>
       </c>
@@ -916,7 +916,7 @@
         <v>43175</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>65</v>
       </c>
@@ -930,7 +930,7 @@
         <v>43175</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -947,7 +947,7 @@
         <v>43183</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -964,7 +964,7 @@
         <v>43183</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>67</v>
       </c>
@@ -981,7 +981,7 @@
         <v>43185</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>71</v>
       </c>

</xml_diff>

<commit_message>
rm old checkpoints and update docs2
</commit_message>
<xml_diff>
--- a/documentation/Sprint 2 Tests.xlsx
+++ b/documentation/Sprint 2 Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnh\Desktop\NCAA-Bracket-Predictor\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A48BCB-CB63-4845-98C1-26AF5792A1AA}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1AC783D-9488-4DCE-A6CE-37CCA47DA5AD}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5628" xr2:uid="{9DF9FD2C-CE41-44D9-B248-E86D16A5E2AD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="74">
   <si>
     <t>Test</t>
   </si>
@@ -252,9 +252,6 @@
   </si>
   <si>
     <t>proves best_points works.</t>
-  </si>
-  <si>
-    <t>########</t>
   </si>
 </sst>
 </file>
@@ -654,8 +651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50E2C35C-2831-4627-8391-15309EF4B4D5}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -664,7 +661,7 @@
     <col min="2" max="2" width="50" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="40.5234375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40" customWidth="1"/>
-    <col min="5" max="5" width="9.1015625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.47265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.75">
@@ -697,8 +694,8 @@
       <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>74</v>
+      <c r="E2" s="2">
+        <v>43167</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">

</xml_diff>